<commit_message>
mad some changes to the report
</commit_message>
<xml_diff>
--- a/prac_3_2/graphs.xlsx
+++ b/prac_3_2/graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62ce1d03d1827cd4/Desktop/FRSKIA001_CLRCAM007_ES3/FRSKIA001_CLRCAM007_ES3/prac_3_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kianf\OneDrive\Desktop\FRSKIA001_CLRCAM007_ES3\FRSKIA001_CLRCAM007_ES3\prac_3_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{0450FC45-E972-CD47-9B1E-DA4FBC376D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE33D9C8-5147-4608-B08B-2A792C0C9799}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D0C026-D5CF-48BA-A193-AA1147A136A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{495A3C41-0290-A44E-B57D-E58F10224CF2}"/>
   </bookViews>
@@ -2709,20 +2709,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of the matrix</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2785,6 +2831,73 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.7397260273972601E-2"/>
+              <c:y val="0.42768099222184619"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2835,7 +2948,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3664,20 +3777,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of matrices being multiplied together</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3740,6 +3894,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.8997263422183551E-2"/>
+              <c:y val="0.42782185509905268"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3790,7 +4007,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4619,20 +4836,96 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of matrices being multiplied together</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4695,6 +4988,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4745,7 +5100,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5574,20 +5929,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of matrices being multiplied together</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5650,6 +6053,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5700,7 +6165,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6529,20 +6994,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of matrices being multiplied together</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6605,6 +7118,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6655,7 +7230,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7484,20 +8059,76 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of matrices being multiplied together</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.25610720297798523"/>
+              <c:y val="0.87744874372803638"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7560,6 +8191,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7610,7 +8303,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13166,15 +13859,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>423334</xdr:colOff>
+      <xdr:colOff>434324</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>43473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
+      <xdr:colOff>49091</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>145073</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13244,13 +13937,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>173566</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>118533</xdr:rowOff>
+      <xdr:rowOff>138944</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>622299</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
+      <xdr:rowOff>37344</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13640,8 +14333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9638D0BC-FA10-DC45-8B84-163D5FF41A31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>